<commit_message>
update documentation of BMP values
</commit_message>
<xml_diff>
--- a/documentation/dbfz_bmp_tests.xlsx
+++ b/documentation/dbfz_bmp_tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shellmann\SimonsHardDriveSpeicher\GIT\ad_meal_prep_control\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483CA774-DF67-4632-8C08-9A2C2A867926}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFAD838-D014-45FC-87DE-68D638807C8E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{FEC59851-A8F1-448C-AC8E-0F026119D9F7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Substrate</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>20-0468</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>S:\Labororganisation\Eudiometer\DBFZ Datensammlung Batchversuche\Datenmatrix_Batchtversuche_DBFZ 03.11..xlsx, Spalte DU</t>
   </si>
 </sst>
 </file>
@@ -406,15 +412,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13097D96-453C-4754-B6F4-2587C6CDF58A}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,8 +438,11 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -441,8 +455,11 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -455,8 +472,11 @@
       <c r="D3" t="s">
         <v>4</v>
       </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -468,6 +488,9 @@
       </c>
       <c r="D4" t="s">
         <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>